<commit_message>
Backend del formulario de contacto y mail enviado a la administración del ecommerce
</commit_message>
<xml_diff>
--- a/Planificación del proyecto/CI6 Equipo 01.xlsx
+++ b/Planificación del proyecto/CI6 Equipo 01.xlsx
@@ -1607,8 +1607,8 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N64" sqref="C64:N64"/>
+    <sheetView topLeftCell="D46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -37719,8 +37719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V62" sqref="V62"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -42292,10 +42292,18 @@
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D82" s="8"/>
+    </row>
+    <row r="83" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D83" s="8"/>
+    </row>
+    <row r="84" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D84" s="8"/>
+    </row>
+    <row r="85" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D85" s="8"/>
+    </row>
     <row r="86" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="87" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="88" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>